<commit_message>
XGBoost open to open included
</commit_message>
<xml_diff>
--- a/lester/Computations.xlsx
+++ b/lester/Computations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/My Passport/Lester/IVLE/DBA4761/FInal Project/bitcoin-forecasting/lester/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022438E8-59EB-1747-8B14-54673712D976}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DEF207-F436-294F-8866-90E7832AF340}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="-19480" windowWidth="28040" windowHeight="16500" xr2:uid="{24170BEC-76B6-E244-8717-6042658E13B1}"/>
+    <workbookView xWindow="3480" yWindow="-19940" windowWidth="27260" windowHeight="16500" xr2:uid="{24170BEC-76B6-E244-8717-6042658E13B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>acutal_cum</t>
+  </si>
+  <si>
+    <t>buyhold_cum</t>
+  </si>
+  <si>
+    <t>trading costs</t>
+  </si>
+  <si>
+    <t>pred_class_shiftdown</t>
+  </si>
+  <si>
+    <t>lag(pred_class, 1, default= 0)</t>
+  </si>
+  <si>
+    <t>Buy 1 share</t>
   </si>
 </sst>
 </file>
@@ -513,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F72B79F-6C75-F14F-8B8E-DB2EB2F732FA}">
-  <dimension ref="A1:V36"/>
+  <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,16 +542,16 @@
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="19.5" customWidth="1"/>
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="9" max="10" width="13" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -561,8 +576,9 @@
       <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -595,8 +611,9 @@
         <f>1+H3</f>
         <v>1.0324737344794652</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -630,7 +647,7 @@
         <v>1.0316596429987452</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -664,7 +681,7 @@
         <v>1.0316596429987452</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="9">
         <v>43104</v>
       </c>
@@ -695,7 +712,7 @@
         <v>1.0451690943848233</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" s="9">
         <v>43105</v>
       </c>
@@ -722,7 +739,7 @@
         <v>1.0451690943848233</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
         <v>43106</v>
       </c>
@@ -737,8 +754,9 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -758,7 +776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="9">
         <v>43101</v>
       </c>
@@ -781,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="9">
         <v>43102</v>
       </c>
@@ -804,7 +822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="9">
         <v>43103</v>
       </c>
@@ -827,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="9">
         <v>43104</v>
       </c>
@@ -850,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B17" s="9">
         <v>43105</v>
       </c>
@@ -873,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B18" s="5">
         <v>43106</v>
       </c>
@@ -885,7 +903,7 @@
       <c r="F18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B23" s="10" t="s">
         <v>13</v>
       </c>
@@ -895,8 +913,11 @@
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -920,25 +941,34 @@
         <v>21</v>
       </c>
       <c r="J24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="N24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="O24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S24">
+      <c r="U24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X24">
         <v>-3.499999999999992E-2</v>
       </c>
-      <c r="U24" t="s">
+      <c r="Z24" t="s">
         <v>14</v>
       </c>
-      <c r="V24" t="s">
+      <c r="AA24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>1</v>
       </c>
@@ -965,29 +995,37 @@
       <c r="I25">
         <v>1</v>
       </c>
-      <c r="J25">
-        <f>I25*F25</f>
-        <v>9.5321855728598859E-2</v>
+      <c r="K25">
+        <f>ABS(I25-J25)*0.0003</f>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="L25">
+        <f>I25*F25-K25</f>
+        <v>9.5021855728598864E-2</v>
+      </c>
+      <c r="O25">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="R25">
+      <c r="U25">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="W25">
         <f>C26/C25-1</f>
         <v>-3.499999999999992E-2</v>
       </c>
-      <c r="S25">
+      <c r="X25">
         <v>9.5321855728598859E-2</v>
       </c>
-      <c r="U25" s="1">
+      <c r="Z25" s="1">
         <v>9.1905997099999998E-2</v>
       </c>
-      <c r="V25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="AA25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>2</v>
       </c>
@@ -1005,7 +1043,7 @@
         <v>9.1905997064732903E-2</v>
       </c>
       <c r="F26">
-        <f t="shared" ref="F26:F34" si="3">C28/C27-1</f>
+        <f t="shared" ref="F26:F32" si="3">C28/C27-1</f>
         <v>3.3035329658045676E-2</v>
       </c>
       <c r="G26">
@@ -1016,28 +1054,39 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <f t="shared" ref="J26:K36" si="5">I26*F26</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <f>ABS(I26-J26)*0.0003</f>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="L26">
-        <f>L25*(1+K26)</f>
-        <v>1</v>
-      </c>
-      <c r="R26">
+        <f t="shared" ref="L26:L34" si="5">I26*F26-K26</f>
+        <v>-2.9999999999999997E-4</v>
+      </c>
+      <c r="O26">
+        <f>O25*(1+N26)</f>
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <f>U25*(1+E26)</f>
+        <v>1.0919059970647329</v>
+      </c>
+      <c r="W26">
         <f>C27/C26-1</f>
         <v>9.5321855728598859E-2</v>
       </c>
-      <c r="S26">
+      <c r="X26">
         <v>3.3035329658045676E-2</v>
       </c>
-      <c r="U26" s="1">
+      <c r="Z26" s="1">
         <v>3.2473734499999997E-2</v>
       </c>
-      <c r="V26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="AA26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>3</v>
       </c>
@@ -1066,31 +1115,43 @@
         <v>1</v>
       </c>
       <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ref="K27:K34" si="7">ABS(I27-J27)*0.0003</f>
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L27">
         <f t="shared" si="5"/>
-        <v>-7.884863832691158E-4</v>
-      </c>
-      <c r="K27">
-        <v>9.5321855728598859E-2</v>
-      </c>
-      <c r="L27">
-        <f t="shared" ref="L27:L34" si="7">L26*(1+K27)</f>
-        <v>1.0953218557285989</v>
-      </c>
-      <c r="R27">
+        <v>-1.0884863832691157E-3</v>
+      </c>
+      <c r="N27">
+        <f>L25</f>
+        <v>9.5021855728598864E-2</v>
+      </c>
+      <c r="O27">
+        <f t="shared" ref="O27:O34" si="8">O26*(1+N27)</f>
+        <v>1.0950218557285989</v>
+      </c>
+      <c r="U27">
+        <f>U26*(1+E27)</f>
+        <v>1.1273642624899487</v>
+      </c>
+      <c r="W27">
         <f>C28/C27-1</f>
         <v>3.3035329658045676E-2</v>
       </c>
-      <c r="S27">
+      <c r="X27">
         <v>-7.884863832691158E-4</v>
       </c>
-      <c r="U27" s="1">
+      <c r="Z27" s="1">
         <v>-7.8848640000000005E-4</v>
       </c>
-      <c r="V27" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="AA27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>4</v>
       </c>
@@ -1119,31 +1180,43 @@
         <v>1</v>
       </c>
       <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L28">
         <f t="shared" si="5"/>
         <v>0.11782612801256254</v>
       </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="7"/>
-        <v>1.0953218557285989</v>
-      </c>
-      <c r="R28">
+      <c r="N28">
+        <f t="shared" ref="N28:N34" si="9">L26</f>
+        <v>-2.9999999999999997E-4</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="8"/>
+        <v>1.0946933491718804</v>
+      </c>
+      <c r="U28">
+        <f>U27*(1+E28)</f>
+        <v>1.1264753511199912</v>
+      </c>
+      <c r="W28">
         <f>C29/C28-1</f>
         <v>-7.884863832691158E-4</v>
       </c>
-      <c r="S28">
+      <c r="X28">
         <v>0.11782612801256254</v>
       </c>
-      <c r="U28" s="1">
+      <c r="Z28" s="1">
         <v>0.11782678839999999</v>
       </c>
-      <c r="V28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="AA28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>5</v>
       </c>
@@ -1172,31 +1245,43 @@
         <v>1</v>
       </c>
       <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L29">
         <f t="shared" si="5"/>
         <v>1.2667776859508928E-2</v>
       </c>
-      <c r="K29">
-        <v>-7.884863832691158E-4</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="7"/>
-        <v>1.0944582093600599</v>
-      </c>
-      <c r="R29">
+      <c r="N29">
+        <f t="shared" si="9"/>
+        <v>-1.0884863832691157E-3</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="8"/>
+        <v>1.0935017903674515</v>
+      </c>
+      <c r="U29">
+        <f>U28*(1+E29)</f>
+        <v>1.2592043239029382</v>
+      </c>
+      <c r="W29">
         <f>C30/C29-1</f>
         <v>0.11782612801256254</v>
       </c>
-      <c r="S29">
+      <c r="X29">
         <v>1.2667776859508928E-2</v>
       </c>
-      <c r="U29" s="1">
+      <c r="Z29" s="1">
         <v>1.3094872400000001E-2</v>
       </c>
-      <c r="V29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="AA29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
         <v>6</v>
       </c>
@@ -1225,31 +1310,43 @@
         <v>0</v>
       </c>
       <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="7"/>
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L30">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K30">
+        <v>-2.9999999999999997E-4</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="9"/>
         <v>0.11782612801256254</v>
       </c>
-      <c r="L30">
-        <f t="shared" si="7"/>
-        <v>1.2234139824405184</v>
-      </c>
-      <c r="R30">
+      <c r="O30">
+        <f t="shared" si="8"/>
+        <v>1.2223448723012531</v>
+      </c>
+      <c r="U30">
+        <f>U29*(1+E30)</f>
+        <v>1.2756934438509275</v>
+      </c>
+      <c r="W30">
         <f>C31/C30-1</f>
         <v>1.2667776859508928E-2</v>
       </c>
-      <c r="S30">
+      <c r="X30">
         <v>-5.6494324316914257E-2</v>
       </c>
-      <c r="U30" s="1">
+      <c r="Z30" s="1">
         <v>-5.9805815499999998E-2</v>
       </c>
-      <c r="V30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="AA30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
         <v>7</v>
       </c>
@@ -1278,31 +1375,43 @@
         <v>0</v>
       </c>
       <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L31">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K31">
+      <c r="N31">
+        <f t="shared" si="9"/>
         <v>1.2667776859508928E-2</v>
       </c>
-      <c r="L31">
-        <f t="shared" si="7"/>
-        <v>1.2389119177768779</v>
-      </c>
-      <c r="R31">
+      <c r="O31">
+        <f t="shared" si="8"/>
+        <v>1.2378292643889304</v>
+      </c>
+      <c r="U31">
+        <f>U30*(1+E31)</f>
+        <v>1.1993995571064187</v>
+      </c>
+      <c r="W31">
         <f>C32/C31-1</f>
         <v>-5.6494324316914257E-2</v>
       </c>
-      <c r="S31">
+      <c r="X31">
         <v>-7.2585102739090801E-2</v>
       </c>
-      <c r="U31" s="1">
+      <c r="Z31" s="1">
         <v>-6.9711523600000005E-2</v>
       </c>
-      <c r="V31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="AA31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
         <v>8</v>
       </c>
@@ -1331,31 +1440,43 @@
         <v>1</v>
       </c>
       <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="7"/>
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L32">
         <f t="shared" si="5"/>
-        <v>-3.9765359843573211E-2</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="7"/>
-        <v>1.2389119177768779</v>
-      </c>
-      <c r="R32">
+        <v>-4.0065359843573213E-2</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="9"/>
+        <v>-2.9999999999999997E-4</v>
+      </c>
+      <c r="O32">
+        <f>O31*(1+N32)</f>
+        <v>1.2374579156096137</v>
+      </c>
+      <c r="U32">
+        <f>U31*(1+E32)</f>
+        <v>1.1157875866316656</v>
+      </c>
+      <c r="W32">
         <f>C33/C32-1</f>
         <v>-7.2585102739090801E-2</v>
       </c>
-      <c r="S32">
+      <c r="X32">
         <v>-3.9765359843573211E-2</v>
       </c>
-      <c r="U32" s="1">
+      <c r="Z32" s="1">
         <v>-3.9765359799999997E-2</v>
       </c>
-      <c r="V32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="AA32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
         <v>9</v>
       </c>
@@ -1380,28 +1501,40 @@
         <v>1</v>
       </c>
       <c r="J33">
-        <f>I33*F33</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L33">
-        <f t="shared" si="7"/>
-        <v>1.2389119177768779</v>
-      </c>
-      <c r="R33">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="8"/>
+        <v>1.2374579156096137</v>
+      </c>
+      <c r="U33">
+        <f>U32*(1+E33)</f>
+        <v>1.0714178917402652</v>
+      </c>
+      <c r="W33">
         <f>C34/C33-1</f>
         <v>-3.9765359843573211E-2</v>
       </c>
-      <c r="U33" s="1">
+      <c r="Z33" s="1">
         <v>3.3777183500000002E-2</v>
       </c>
-      <c r="V33" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="AA33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
         <v>10</v>
       </c>
@@ -1426,29 +1559,171 @@
         <v>1</v>
       </c>
       <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K34">
-        <v>-3.9765359843573211E-2</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="7"/>
-        <v>1.1896461395519891</v>
-      </c>
-      <c r="U34" s="1">
+      <c r="N34">
+        <f t="shared" si="9"/>
+        <v>-4.0065359843573213E-2</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="8"/>
+        <v>1.1878787189294366</v>
+      </c>
+      <c r="U34">
+        <f>U33*(1+E34)</f>
+        <v>1.1076073704513958</v>
+      </c>
+      <c r="Z34" s="1">
         <v>-0.110556601</v>
       </c>
-      <c r="V34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="AA34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="F36" t="s">
         <v>16</v>
       </c>
-      <c r="K36" t="s">
+      <c r="M36" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="J37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="C41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="C42" s="1">
+        <v>13880</v>
+      </c>
+      <c r="D42" s="1">
+        <v>13443.41</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <f>ABS(F42-G42)*0.0003</f>
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="C43" s="1">
+        <v>13394.2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>14678.94</v>
+      </c>
+      <c r="E43">
+        <f>D43/D42-1</f>
+        <v>9.1905997064732903E-2</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <f>ABS(F43-G43)*0.0003</f>
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="C44" s="1">
+        <v>14670.96</v>
+      </c>
+      <c r="D44" s="1">
+        <v>15155.62</v>
+      </c>
+      <c r="E44">
+        <f t="shared" ref="E44:E45" si="10">D44/D43-1</f>
+        <v>3.2473734479465222E-2</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <f t="shared" ref="H44:H51" si="11">ABS(F44-G44)*0.0003</f>
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="C45" s="1">
+        <v>15155.62</v>
+      </c>
+      <c r="D45" s="1">
+        <v>15143.67</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="10"/>
+        <v>-7.884863832691158E-4</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F49" t="s">
+        <v>29</v>
+      </c>
+      <c r="G49">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>6000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>